<commit_message>
Expand sample scripts to 100 sentences each and update resources pages
</commit_message>
<xml_diff>
--- a/assets/files/samples/basic_korean.xlsx
+++ b/assets/files/samples/basic_korean.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,15 +412,15 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>안녕하세요!</v>
+        <v>안녕하세요.</v>
       </c>
       <c r="B2" t="str">
-        <v>Hello!</v>
+        <v>Hello.</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>반가워요.</v>
+        <v>처음 뵙겠습니다.</v>
       </c>
       <c r="B3" t="str">
         <v>Nice to meet you.</v>
@@ -428,231 +428,791 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>감사합니다.</v>
+        <v>오랜만이에요.</v>
       </c>
       <c r="B4" t="str">
-        <v>Thank you.</v>
+        <v>Long time no see.</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>죄송합니다.</v>
+        <v>어떻게 지내세요?</v>
       </c>
       <c r="B5" t="str">
-        <v>I'm sorry.</v>
+        <v>How are you doing?</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>얼마예요?</v>
+        <v>잘 지내요.</v>
       </c>
       <c r="B6" t="str">
-        <v>How much is this?</v>
+        <v>I'm doing well.</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>맛있어요.</v>
+        <v>만나서 반가워요.</v>
       </c>
       <c r="B7" t="str">
-        <v>It's delicious.</v>
+        <v>Glad to meet you.</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>사랑해요.</v>
+        <v>감사합니다.</v>
       </c>
       <c r="B8" t="str">
-        <v>I love you.</v>
+        <v>Thank you.</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>잠시만요.</v>
+        <v>천만에요.</v>
       </c>
       <c r="B9" t="str">
-        <v>Just a moment.</v>
+        <v>You're welcome.</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>화이팅!</v>
+        <v>죄송합니다.</v>
       </c>
       <c r="B10" t="str">
-        <v>Cheer up! / Good luck!</v>
+        <v>I'm sorry.</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>안녕히 가세요.</v>
+        <v>괜찮아요.</v>
       </c>
       <c r="B11" t="str">
-        <v>Goodbye. (to someone leaving)</v>
+        <v>It's okay.</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>안녕히 계세요.</v>
+        <v>실례합니다.</v>
       </c>
       <c r="B12" t="str">
-        <v>Goodbye. (to someone staying)</v>
+        <v>Excuse me.</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>잘 자요.</v>
+        <v>잠시만요.</v>
       </c>
       <c r="B13" t="str">
-        <v>Good night.</v>
+        <v>Just a moment.</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>배가 고파요.</v>
+        <v>저기요.</v>
       </c>
       <c r="B14" t="str">
-        <v>I'm hungry.</v>
+        <v>Excuse me (to call someone).</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>어디예요?</v>
+        <v>네.</v>
       </c>
       <c r="B15" t="str">
-        <v>Where are you?</v>
+        <v>Yes.</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>화장실 어디예요?</v>
+        <v>아니요.</v>
       </c>
       <c r="B16" t="str">
-        <v>Where is the bathroom?</v>
+        <v>No.</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>도와주세요.</v>
+        <v>아마도요.</v>
       </c>
       <c r="B17" t="str">
-        <v>Help me.</v>
+        <v>Maybe.</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>괜찮아요.</v>
+        <v>물론이죠.</v>
       </c>
       <c r="B18" t="str">
-        <v>I'm okay.</v>
+        <v>Of course.</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>축하해요!</v>
+        <v>부탁합니다.</v>
       </c>
       <c r="B19" t="str">
-        <v>Congratulations!</v>
+        <v>Please.</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>생일 축하해요.</v>
+        <v>도와주세요.</v>
       </c>
       <c r="B20" t="str">
-        <v>Happy birthday.</v>
+        <v>Help me.</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>이름이 뭐예요?</v>
+        <v>이해했어요.</v>
       </c>
       <c r="B21" t="str">
-        <v>What is your name?</v>
+        <v>I understand.</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>제 이름은 ...입니다.</v>
+        <v>이해 못 했어요.</v>
       </c>
       <c r="B22" t="str">
-        <v>My name is ...</v>
+        <v>I don't understand.</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>한국 사람이에요?</v>
+        <v>다시 말해주세요.</v>
       </c>
       <c r="B23" t="str">
-        <v>Are you Korean?</v>
+        <v>Please say it again.</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>영어 할 수 있어요?</v>
+        <v>천천히 말해주세요.</v>
       </c>
       <c r="B24" t="str">
-        <v>Can you speak English?</v>
+        <v>Please speak slowly.</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>좋아요.</v>
+        <v>영어 할 수 있어요?</v>
       </c>
       <c r="B25" t="str">
-        <v>I like it. / Good.</v>
+        <v>Can you speak English?</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>싫어요.</v>
+        <v>한국어 조금 해요.</v>
       </c>
       <c r="B26" t="str">
-        <v>I don't like it.</v>
+        <v>I speak a little Korean.</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>진짜요?</v>
+        <v>이름이 뭐예요?</v>
       </c>
       <c r="B27" t="str">
-        <v>Really?</v>
+        <v>What is your name?</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>몰라요.</v>
+        <v>제 이름은 ...입니다.</v>
       </c>
       <c r="B28" t="str">
-        <v>I don't know.</v>
+        <v>My name is ...</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>알아요.</v>
+        <v>어디서 오셨어요?</v>
       </c>
       <c r="B29" t="str">
-        <v>I know.</v>
+        <v>Where are you from?</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>천만에요.</v>
+        <v>저는 미국에서 왔어요.</v>
       </c>
       <c r="B30" t="str">
-        <v>You're welcome.</v>
+        <v>I am from the USA.</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>다음에 봐요.</v>
+        <v>몇 살이세요?</v>
       </c>
       <c r="B31" t="str">
-        <v>See you next time.</v>
+        <v>How old are you?</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>직업이 뭐예요?</v>
+      </c>
+      <c r="B32" t="str">
+        <v>What is your job?</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>학생이에요.</v>
+      </c>
+      <c r="B33" t="str">
+        <v>I am a student.</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>회사원이에요.</v>
+      </c>
+      <c r="B34" t="str">
+        <v>I am an office worker.</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>취미가 뭐예요?</v>
+      </c>
+      <c r="B35" t="str">
+        <v>What are your hobbies?</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>저는 영화 보는 걸 좋아해요.</v>
+      </c>
+      <c r="B36" t="str">
+        <v>I like watching movies.</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>오늘 날씨가 좋네요.</v>
+      </c>
+      <c r="B37" t="str">
+        <v>The weather is good today.</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>비가 오네요.</v>
+      </c>
+      <c r="B38" t="str">
+        <v>It's raining.</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>추워요.</v>
+      </c>
+      <c r="B39" t="str">
+        <v>It's cold.</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>더워요.</v>
+      </c>
+      <c r="B40" t="str">
+        <v>It's hot.</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>지금 몇 시예요?</v>
+      </c>
+      <c r="B41" t="str">
+        <v>What time is it now?</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>배고파요.</v>
+      </c>
+      <c r="B42" t="str">
+        <v>I'm hungry.</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>배불러요.</v>
+      </c>
+      <c r="B43" t="str">
+        <v>I'm full.</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>목 말라요.</v>
+      </c>
+      <c r="B44" t="str">
+        <v>I'm thirsty.</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>맛있어요.</v>
+      </c>
+      <c r="B45" t="str">
+        <v>It's delicious.</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>맛없어요.</v>
+      </c>
+      <c r="B46" t="str">
+        <v>It's not delicious.</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>잘 먹겠습니다.</v>
+      </c>
+      <c r="B47" t="str">
+        <v>I will eat well (Bon appétit).</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>잘 먹었습니다.</v>
+      </c>
+      <c r="B48" t="str">
+        <v>I ate well (Thank you for the meal).</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>메뉴판 주세요.</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Menu please.</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>이거 주세요.</v>
+      </c>
+      <c r="B50" t="str">
+        <v>This one please.</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>물 좀 주세요.</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Water please.</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>계산해 주세요.</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Check please.</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>영수증 주세요.</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Receipt please.</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>화장실이 어디예요?</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Where is the bathroom?</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>입구는 어디예요?</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Where is the entrance?</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>출구는 어디예요?</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Where is the exit?</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>왼쪽으로 가세요.</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Go left.</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>오른쪽으로 가세요.</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Go right.</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>쭉 가세요.</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Go straight.</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>여기서 세워주세요.</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Stop here please.</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>얼마예요?</v>
+      </c>
+      <c r="B61" t="str">
+        <v>How much is it?</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>너무 비싸요.</v>
+      </c>
+      <c r="B62" t="str">
+        <v>It's too expensive.</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>깎아주세요.</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Please give me a discount.</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>카드로 계산할게요.</v>
+      </c>
+      <c r="B64" t="str">
+        <v>I will pay by card.</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>현금으로 계산할게요.</v>
+      </c>
+      <c r="B65" t="str">
+        <v>I will pay by cash.</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>환불해 주세요.</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Please refund it.</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>교환해 주세요.</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Please exchange it.</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>이거 입어봐도 되나요?</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Can I try this on?</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>사이즈가 안 맞아요.</v>
+      </c>
+      <c r="B69" t="str">
+        <v>The size doesn't fit.</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>더 큰 사이즈 있어요?</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Do you have a bigger size?</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>더 작은 사이즈 있어요?</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Do you have a smaller size?</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>어떤 색깔 좋아해요?</v>
+      </c>
+      <c r="B72" t="str">
+        <v>What color do you like?</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>파란색 좋아해요.</v>
+      </c>
+      <c r="B73" t="str">
+        <v>I like blue.</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>생일 축하해요.</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Happy birthday.</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>축하해요!</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Congratulations!</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>새해 복 많이 받으세요.</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Happy New Year.</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>메리 크리스마스.</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Merry Christmas.</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>사랑해요.</v>
+      </c>
+      <c r="B78" t="str">
+        <v>I love you.</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>보고 싶어요.</v>
+      </c>
+      <c r="B79" t="str">
+        <v>I miss you.</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>좋아해요.</v>
+      </c>
+      <c r="B80" t="str">
+        <v>I like you.</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>결혼해 줄래?</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Will you marry me?</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>헤어지자.</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Let's break up.</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>정말요?</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Really?</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>거짓말 하지 마세요.</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Don't lie.</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>약속해요.</v>
+      </c>
+      <c r="B85" t="str">
+        <v>I promise.</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>비밀이에요.</v>
+      </c>
+      <c r="B86" t="str">
+        <v>It's a secret.</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>걱정하지 마세요.</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Don't worry.</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>힘내세요.</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Cheer up.</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>수고하셨습니다.</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Good job.</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>피곤해요.</v>
+      </c>
+      <c r="B90" t="str">
+        <v>I'm tired.</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>아파요.</v>
+      </c>
+      <c r="B91" t="str">
+        <v>I'm sick/It hurts.</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>병원에 가야 해요.</v>
+      </c>
+      <c r="B92" t="str">
+        <v>I need to go to the hospital.</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>약국이 어디예요?</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Where is the pharmacy?</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>머리가 아파요.</v>
+      </c>
+      <c r="B94" t="str">
+        <v>I have a headache.</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>배가 아파요.</v>
+      </c>
+      <c r="B95" t="str">
+        <v>I have a stomachache.</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>감기 걸렸어요.</v>
+      </c>
+      <c r="B96" t="str">
+        <v>I caught a cold.</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>조심하세요.</v>
+      </c>
+      <c r="B97" t="str">
+        <v>Be careful.</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>위험해요.</v>
+      </c>
+      <c r="B98" t="str">
+        <v>It's dangerous.</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>도와드릴까요?</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Can I help you?</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>무슨 일이에요?</v>
+      </c>
+      <c r="B100" t="str">
+        <v>What happened?</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>재미있어요.</v>
+      </c>
+      <c r="B101" t="str">
+        <v>It's fun.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B31"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B101"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>